<commit_message>
energyic_UART updates and excel sheet
insert some #define in UART .h
create new functions

Update excel sheet
</commit_message>
<xml_diff>
--- a/doc/Energy setpoint calculator.xlsx
+++ b/doc/Energy setpoint calculator.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20325"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Downloads\-\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99DCB3BD-14CE-44B9-A56E-1A33EAD8DD3F}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16395" windowHeight="10530"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8130" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="CS1" sheetId="2" r:id="rId2"/>
+    <sheet name="CS2" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="GL">Sheet1!$B$24</definedName>
@@ -26,17 +27,24 @@
     <definedName name="Vratio">Sheet1!$B$1</definedName>
     <definedName name="VU">Sheet1!$B$26</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179021"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Wendland, Ryan</author>
   </authors>
   <commentList>
-    <comment ref="A5" authorId="0" shapeId="0">
+    <comment ref="A5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -60,7 +68,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A6" authorId="0" shapeId="0">
+    <comment ref="A6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -84,7 +92,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A7" authorId="0" shapeId="0">
+    <comment ref="A7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -109,7 +117,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A8" authorId="0" shapeId="0">
+    <comment ref="A8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
@@ -133,7 +141,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A9" authorId="0" shapeId="0">
+    <comment ref="A9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
       <text>
         <r>
           <rPr>
@@ -157,7 +165,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A10" authorId="0" shapeId="0">
+    <comment ref="A10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
       <text>
         <r>
           <rPr>
@@ -181,7 +189,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A11" authorId="0" shapeId="0">
+    <comment ref="A11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
       <text>
         <r>
           <rPr>
@@ -205,7 +213,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A12" authorId="0" shapeId="0">
+    <comment ref="A12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
       <text>
         <r>
           <rPr>
@@ -234,7 +242,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="135">
   <si>
     <t>Voltage ratio</t>
   </si>
@@ -847,15 +855,129 @@
   <si>
     <t>Impulse converter</t>
   </si>
+  <si>
+    <t>Reg</t>
+  </si>
+  <si>
+    <t>Hex Value</t>
+  </si>
+  <si>
+    <t>2A</t>
+  </si>
+  <si>
+    <t>2B</t>
+  </si>
+  <si>
+    <t>Decimal H</t>
+  </si>
+  <si>
+    <t>Decimal L</t>
+  </si>
+  <si>
+    <t>H2x</t>
+  </si>
+  <si>
+    <t>L2x</t>
+  </si>
+  <si>
+    <t>1D39</t>
+  </si>
+  <si>
+    <t>0000</t>
+  </si>
+  <si>
+    <t>08BD</t>
+  </si>
+  <si>
+    <t>0AEC</t>
+  </si>
+  <si>
+    <t>9422</t>
+  </si>
+  <si>
+    <t>L2C</t>
+  </si>
+  <si>
+    <t>H2C</t>
+  </si>
+  <si>
+    <t>Reg 2C</t>
+  </si>
+  <si>
+    <t>31</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>33</t>
+  </si>
+  <si>
+    <t>34</t>
+  </si>
+  <si>
+    <t>35</t>
+  </si>
+  <si>
+    <t>36</t>
+  </si>
+  <si>
+    <t>37</t>
+  </si>
+  <si>
+    <t>38</t>
+  </si>
+  <si>
+    <t>39</t>
+  </si>
+  <si>
+    <t>3A</t>
+  </si>
+  <si>
+    <t>3B</t>
+  </si>
+  <si>
+    <t>D464</t>
+  </si>
+  <si>
+    <t>6E49</t>
+  </si>
+  <si>
+    <t>H3C</t>
+  </si>
+  <si>
+    <t>L3C</t>
+  </si>
+  <si>
+    <t>Reg 3C</t>
+  </si>
+  <si>
+    <t>7530</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Ps.: unlock just if necessary</t>
+  </si>
+  <si>
+    <t>Ps2.: change just the green numbers based on register values</t>
+  </si>
+  <si>
+    <t>00B9</t>
+  </si>
+  <si>
+    <t>C1F3</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="16">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -937,6 +1059,39 @@
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Cambia Math"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1028,7 +1183,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1080,16 +1235,45 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="Calculation" xfId="3" builtinId="22"/>
-    <cellStyle name="Input" xfId="1" builtinId="20"/>
+    <cellStyle name="Cálculo" xfId="3" builtinId="22"/>
+    <cellStyle name="Entrada" xfId="1" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Output" xfId="2" builtinId="21"/>
+    <cellStyle name="Saída" xfId="2" builtinId="21"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1118,7 +1302,13 @@
       <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="3" name="TextBox 2"/>
+            <xdr:cNvPr id="3" name="TextBox 2">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
             <xdr:cNvSpPr txBox="1"/>
           </xdr:nvSpPr>
           <xdr:spPr>
@@ -1736,7 +1926,13 @@
       <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="5" name="TextBox 4"/>
+            <xdr:cNvPr id="5" name="TextBox 4">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
             <xdr:cNvSpPr txBox="1"/>
           </xdr:nvSpPr>
           <xdr:spPr>
@@ -2154,7 +2350,13 @@
       <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="6" name="TextBox 5"/>
+            <xdr:cNvPr id="6" name="TextBox 5">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
             <xdr:cNvSpPr txBox="1"/>
           </xdr:nvSpPr>
           <xdr:spPr>
@@ -2557,7 +2759,13 @@
       <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="2" name="TextBox 1"/>
+            <xdr:cNvPr id="2" name="TextBox 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
             <xdr:cNvSpPr txBox="1"/>
           </xdr:nvSpPr>
           <xdr:spPr>
@@ -3028,7 +3236,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -3347,12 +3555,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="B57" sqref="B57"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -3364,7 +3570,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="18">
-      <c r="A1" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="6">
@@ -3431,12 +3637,12 @@
       <c r="A5" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="24" t="s">
+      <c r="B5" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="C5" s="24"/>
-      <c r="D5" s="24"/>
-      <c r="E5" s="24"/>
+      <c r="C5" s="35"/>
+      <c r="D5" s="35"/>
+      <c r="E5" s="35"/>
       <c r="F5" s="10" t="str">
         <f>LEFT(B5,FIND(":",B5)-1)</f>
         <v>100</v>
@@ -3466,12 +3672,12 @@
       <c r="A6" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="24" t="s">
+      <c r="B6" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="C6" s="24"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="35"/>
       <c r="F6" s="10" t="str">
         <f t="shared" ref="F6:F12" si="0">LEFT(B6,FIND(":",B6)-1)</f>
         <v>10</v>
@@ -3498,12 +3704,12 @@
       <c r="A7" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="24" t="s">
+      <c r="B7" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="C7" s="24"/>
-      <c r="D7" s="24"/>
-      <c r="E7" s="24"/>
+      <c r="C7" s="35"/>
+      <c r="D7" s="35"/>
+      <c r="E7" s="35"/>
       <c r="F7" s="10" t="str">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -3516,12 +3722,12 @@
       <c r="A8" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="24" t="s">
+      <c r="B8" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="C8" s="24"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="24"/>
+      <c r="C8" s="35"/>
+      <c r="D8" s="35"/>
+      <c r="E8" s="35"/>
       <c r="F8" s="10" t="str">
         <f t="shared" si="0"/>
         <v>00</v>
@@ -3534,12 +3740,12 @@
       <c r="A9" t="s">
         <v>27</v>
       </c>
-      <c r="B9" s="23" t="s">
+      <c r="B9" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="23"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="23"/>
+      <c r="C9" s="34"/>
+      <c r="D9" s="34"/>
+      <c r="E9" s="34"/>
       <c r="F9" s="10" t="str">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3552,12 +3758,12 @@
       <c r="A10" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="23" t="s">
+      <c r="B10" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="C10" s="23"/>
-      <c r="D10" s="23"/>
-      <c r="E10" s="23"/>
+      <c r="C10" s="34"/>
+      <c r="D10" s="34"/>
+      <c r="E10" s="34"/>
       <c r="F10" s="10" t="str">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3570,12 +3776,12 @@
       <c r="A11" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="23" t="s">
+      <c r="B11" s="34" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="23"/>
-      <c r="D11" s="23"/>
-      <c r="E11" s="23"/>
+      <c r="C11" s="34"/>
+      <c r="D11" s="34"/>
+      <c r="E11" s="34"/>
       <c r="F11" s="10" t="str">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -3588,12 +3794,12 @@
       <c r="A12" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="23" t="s">
+      <c r="B12" s="34" t="s">
         <v>37</v>
       </c>
-      <c r="C12" s="23"/>
-      <c r="D12" s="23"/>
-      <c r="E12" s="23"/>
+      <c r="C12" s="34"/>
+      <c r="D12" s="34"/>
+      <c r="E12" s="34"/>
       <c r="F12" s="10" t="str">
         <f t="shared" si="0"/>
         <v>0010</v>
@@ -4254,28 +4460,28 @@
     <mergeCell ref="B8:E8"/>
   </mergeCells>
   <dataValidations disablePrompts="1" count="8">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9:E9">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9:E9" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"0: Fwd or rev energy pulse output, 1: Absolute energy pulse output"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B10:E10">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B10:E10" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"0: Fwd or rev reactive energy pulse output, 1: Absolute reactive energy pulse output"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11:E11">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11:E11" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"00: Positive zero-crossing, 01: Negative zero-crossing, 10: All zero crossing, 11: No zero-crossing"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:E5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:E5" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>"100: Gain 1,000: Gain 4,001: Gain 8,010: Gain 16,011: Gain 24"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6:E6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6:E6" xr:uid="{00000000-0002-0000-0000-000004000000}">
       <formula1>"10: Gain 1, 00: Gain 2, 01: Gain 4"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7:E7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7:E7" xr:uid="{00000000-0002-0000-0000-000005000000}">
       <formula1>"1: Meter on L line,0: Meter on N line"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8:E8">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8:E8" xr:uid="{00000000-0002-0000-0000-000006000000}">
       <formula1>"00: HPF1 and HPF0,01: HPF1 and !HPF0,10: !HPF1 and HPF0,11: !HPF1 and !HPF0"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B12:E12">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B12:E12" xr:uid="{00000000-0002-0000-0000-000007000000}">
       <formula1>"0000: 12.5%,0001: 6.25%,0010: 3.125%,0011: 1.5625%,0100: 1%,0101: 2%,0110: 3%,0111: 4%,1000: 5%,1001: 6%,1010: 7%,1011: 8%,1100: 9%,1101: 10%,1110: 11%,1111: 12%"</formula1>
     </dataValidation>
   </dataValidations>
@@ -4287,25 +4493,719 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="B2:M22"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="2" width="9.140625" style="27"/>
+    <col min="3" max="3" width="10" style="27" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.5703125" style="27" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="27"/>
+    <col min="6" max="6" width="12.42578125" style="27" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="27"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:13">
+      <c r="B2" s="26" t="s">
+        <v>97</v>
+      </c>
+      <c r="C2" s="26" t="s">
+        <v>98</v>
+      </c>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26" t="s">
+        <v>103</v>
+      </c>
+      <c r="F2" s="26" t="s">
+        <v>104</v>
+      </c>
+      <c r="L2" s="33" t="s">
+        <v>101</v>
+      </c>
+      <c r="M2" s="33" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="3" spans="2:13">
+      <c r="B3" s="28">
+        <v>21</v>
+      </c>
+      <c r="C3" s="24" t="s">
+        <v>133</v>
+      </c>
+      <c r="E3" s="23" t="str">
+        <f>DEC2HEX(HEX2DEC(LEFT($C3,2)), 2)</f>
+        <v>00</v>
+      </c>
+      <c r="F3" s="23" t="str">
+        <f>DEC2HEX(HEX2DEC(RIGHT($C3,2)),2)</f>
+        <v>B9</v>
+      </c>
+      <c r="L3" s="27">
+        <f>HEX2DEC(E3)</f>
+        <v>0</v>
+      </c>
+      <c r="M3" s="27">
+        <f>HEX2DEC(F3)</f>
+        <v>185</v>
+      </c>
+    </row>
+    <row r="4" spans="2:13">
+      <c r="B4" s="28">
+        <v>22</v>
+      </c>
+      <c r="C4" s="25" t="s">
+        <v>134</v>
+      </c>
+      <c r="E4" s="23" t="str">
+        <f t="shared" ref="E4:E13" si="0">DEC2HEX(HEX2DEC(LEFT($C4,2)), 2)</f>
+        <v>C1</v>
+      </c>
+      <c r="F4" s="23" t="str">
+        <f t="shared" ref="F4:F13" si="1">DEC2HEX(HEX2DEC(RIGHT($C4,2)),2)</f>
+        <v>F3</v>
+      </c>
+      <c r="L4" s="27">
+        <f>HEX2DEC(E4)</f>
+        <v>193</v>
+      </c>
+      <c r="M4" s="27">
+        <f>HEX2DEC(F4)</f>
+        <v>243</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13">
+      <c r="B5" s="28">
+        <v>23</v>
+      </c>
+      <c r="C5" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="E5" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v>1D</v>
+      </c>
+      <c r="F5" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v>39</v>
+      </c>
+      <c r="L5" s="27">
+        <f t="shared" ref="L5:M13" si="2">HEX2DEC(E5)</f>
+        <v>29</v>
+      </c>
+      <c r="M5" s="27">
+        <f t="shared" si="2"/>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13">
+      <c r="B6" s="28">
+        <v>24</v>
+      </c>
+      <c r="C6" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="E6" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v>00</v>
+      </c>
+      <c r="F6" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v>00</v>
+      </c>
+      <c r="L6" s="27">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M6" s="27">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13">
+      <c r="B7" s="28">
+        <v>25</v>
+      </c>
+      <c r="C7" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="E7" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v>00</v>
+      </c>
+      <c r="F7" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v>00</v>
+      </c>
+      <c r="L7" s="27">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M7" s="27">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13">
+      <c r="B8" s="28">
+        <v>26</v>
+      </c>
+      <c r="C8" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="E8" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v>00</v>
+      </c>
+      <c r="F8" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v>00</v>
+      </c>
+      <c r="L8" s="27">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M8" s="27">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13">
+      <c r="B9" s="28">
+        <v>27</v>
+      </c>
+      <c r="C9" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="E9" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v>08</v>
+      </c>
+      <c r="F9" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v>BD</v>
+      </c>
+      <c r="L9" s="27">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="M9" s="27">
+        <f t="shared" si="2"/>
+        <v>189</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13">
+      <c r="B10" s="28">
+        <v>28</v>
+      </c>
+      <c r="C10" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="E10" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v>00</v>
+      </c>
+      <c r="F10" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v>00</v>
+      </c>
+      <c r="L10" s="27">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M10" s="27">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13">
+      <c r="B11" s="28">
+        <v>29</v>
+      </c>
+      <c r="C11" s="24" t="s">
+        <v>108</v>
+      </c>
+      <c r="E11" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v>0A</v>
+      </c>
+      <c r="F11" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v>EC</v>
+      </c>
+      <c r="L11" s="27">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="M11" s="27">
+        <f t="shared" si="2"/>
+        <v>236</v>
+      </c>
+    </row>
+    <row r="12" spans="2:13">
+      <c r="B12" s="28" t="s">
+        <v>99</v>
+      </c>
+      <c r="C12" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="E12" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v>00</v>
+      </c>
+      <c r="F12" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v>00</v>
+      </c>
+      <c r="L12" s="27">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M12" s="27">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:13">
+      <c r="B13" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="C13" s="24" t="s">
+        <v>109</v>
+      </c>
+      <c r="E13" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v>94</v>
+      </c>
+      <c r="F13" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+      <c r="L13" s="27">
+        <f t="shared" si="2"/>
+        <v>148</v>
+      </c>
+      <c r="M13" s="27">
+        <f t="shared" si="2"/>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="2:13">
+      <c r="E15" s="26" t="s">
+        <v>111</v>
+      </c>
+      <c r="F15" s="29" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="16" spans="2:13">
+      <c r="E16" s="23" t="str">
+        <f>DEC2HEX(_xlfn.BITXOR(_xlfn.BITXOR(_xlfn.BITXOR(_xlfn.BITXOR(_xlfn.BITXOR(_xlfn.BITXOR(_xlfn.BITXOR(_xlfn.BITXOR(_xlfn.BITXOR(_xlfn.BITXOR(_xlfn.BITXOR(_xlfn.BITXOR(_xlfn.BITXOR(_xlfn.BITXOR(_xlfn.BITXOR(_xlfn.BITXOR(_xlfn.BITXOR(_xlfn.BITXOR(_xlfn.BITXOR(_xlfn.BITXOR(_xlfn.BITXOR(L3,L4),L5),L6),L7),L8),L9),L10),L11),L12),L13),M3),M4),M5),M6),M7),M8),M9),M10),M11),M12),M13),2)</f>
+        <v>4A</v>
+      </c>
+      <c r="F16" s="23" t="str">
+        <f>DEC2HEX(MOD(SUM(L3:M13), 256))</f>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6">
+      <c r="E18" s="27" t="s">
+        <v>112</v>
+      </c>
+      <c r="F18" s="30" t="str">
+        <f>"0x"&amp;E16&amp;F16</f>
+        <v>0x4A34</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6">
+      <c r="B19" s="31"/>
+    </row>
+    <row r="20" spans="2:6">
+      <c r="B20" s="32" t="s">
+        <v>130</v>
+      </c>
+      <c r="C20" s="32">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6">
+      <c r="B21" s="32" t="s">
+        <v>131</v>
+      </c>
+      <c r="C21" s="32"/>
+    </row>
+    <row r="22" spans="2:6">
+      <c r="B22" s="32" t="s">
+        <v>132</v>
+      </c>
+      <c r="C22" s="32"/>
+    </row>
+  </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="hXuS+rbd6lffaELnNnjWLSE9Rj8CScJyf+Y75HSHG4mlYyPVdWZINQvHmYJbuN4LQKaTEd4cuDgWbAkKK4ojHA==" saltValue="sbQdwX/EmdsH9NM5J8/AVA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9545B51A-CCD6-4BD2-87D0-B5DB2E7BA0B7}">
+  <dimension ref="B2:M22"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="2" width="9.140625" style="27"/>
+    <col min="3" max="3" width="10" style="27" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.5703125" style="27" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="27"/>
+    <col min="6" max="6" width="12.42578125" style="27" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="27"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:13">
+      <c r="B2" s="26" t="s">
+        <v>97</v>
+      </c>
+      <c r="C2" s="26" t="s">
+        <v>98</v>
+      </c>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26" t="s">
+        <v>103</v>
+      </c>
+      <c r="F2" s="26" t="s">
+        <v>104</v>
+      </c>
+      <c r="L2" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="M2" s="27" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="3" spans="2:13">
+      <c r="B3" s="28" t="s">
+        <v>113</v>
+      </c>
+      <c r="C3" s="24" t="s">
+        <v>124</v>
+      </c>
+      <c r="E3" s="23" t="str">
+        <f>DEC2HEX(HEX2DEC(LEFT($C3,2)), 2)</f>
+        <v>D4</v>
+      </c>
+      <c r="F3" s="23" t="str">
+        <f>DEC2HEX(HEX2DEC(RIGHT($C3,2)),2)</f>
+        <v>64</v>
+      </c>
+      <c r="L3" s="27">
+        <f>HEX2DEC(E3)</f>
+        <v>212</v>
+      </c>
+      <c r="M3" s="27">
+        <f>HEX2DEC(F3)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="2:13">
+      <c r="B4" s="28" t="s">
+        <v>114</v>
+      </c>
+      <c r="C4" s="25" t="s">
+        <v>125</v>
+      </c>
+      <c r="E4" s="23" t="str">
+        <f t="shared" ref="E4:E13" si="0">DEC2HEX(HEX2DEC(LEFT($C4,2)), 2)</f>
+        <v>6E</v>
+      </c>
+      <c r="F4" s="23" t="str">
+        <f t="shared" ref="F4:F13" si="1">DEC2HEX(HEX2DEC(RIGHT($C4,2)),2)</f>
+        <v>49</v>
+      </c>
+      <c r="L4" s="27">
+        <f>HEX2DEC(E4)</f>
+        <v>110</v>
+      </c>
+      <c r="M4" s="27">
+        <f>HEX2DEC(F4)</f>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13">
+      <c r="B5" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="C5" s="24" t="s">
+        <v>129</v>
+      </c>
+      <c r="E5" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v>75</v>
+      </c>
+      <c r="F5" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="L5" s="27">
+        <f t="shared" ref="L5:M13" si="2">HEX2DEC(E5)</f>
+        <v>117</v>
+      </c>
+      <c r="M5" s="27">
+        <f t="shared" si="2"/>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13">
+      <c r="B6" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="C6" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="E6" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v>00</v>
+      </c>
+      <c r="F6" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v>00</v>
+      </c>
+      <c r="L6" s="27">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M6" s="27">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13">
+      <c r="B7" s="28" t="s">
+        <v>117</v>
+      </c>
+      <c r="C7" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="E7" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v>00</v>
+      </c>
+      <c r="F7" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v>00</v>
+      </c>
+      <c r="L7" s="27">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M7" s="27">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13">
+      <c r="B8" s="28" t="s">
+        <v>118</v>
+      </c>
+      <c r="C8" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="E8" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v>00</v>
+      </c>
+      <c r="F8" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v>00</v>
+      </c>
+      <c r="L8" s="27">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M8" s="27">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13">
+      <c r="B9" s="28" t="s">
+        <v>119</v>
+      </c>
+      <c r="C9" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="E9" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v>00</v>
+      </c>
+      <c r="F9" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v>00</v>
+      </c>
+      <c r="L9" s="27">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M9" s="27">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13">
+      <c r="B10" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="C10" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="E10" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v>00</v>
+      </c>
+      <c r="F10" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v>00</v>
+      </c>
+      <c r="L10" s="27">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M10" s="27">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13">
+      <c r="B11" s="28" t="s">
+        <v>121</v>
+      </c>
+      <c r="C11" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="E11" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v>00</v>
+      </c>
+      <c r="F11" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v>00</v>
+      </c>
+      <c r="L11" s="27">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M11" s="27">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:13">
+      <c r="B12" s="28" t="s">
+        <v>122</v>
+      </c>
+      <c r="C12" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="E12" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v>00</v>
+      </c>
+      <c r="F12" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v>00</v>
+      </c>
+      <c r="L12" s="27">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M12" s="27">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:13">
+      <c r="B13" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="C13" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="E13" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v>00</v>
+      </c>
+      <c r="F13" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v>00</v>
+      </c>
+      <c r="L13" s="27">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M13" s="27">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="2:13">
+      <c r="E15" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="F15" s="29" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="16" spans="2:13">
+      <c r="E16" s="23" t="str">
+        <f>DEC2HEX(_xlfn.BITXOR(_xlfn.BITXOR(_xlfn.BITXOR(_xlfn.BITXOR(_xlfn.BITXOR(_xlfn.BITXOR(_xlfn.BITXOR(_xlfn.BITXOR(_xlfn.BITXOR(_xlfn.BITXOR(_xlfn.BITXOR(_xlfn.BITXOR(_xlfn.BITXOR(_xlfn.BITXOR(_xlfn.BITXOR(_xlfn.BITXOR(_xlfn.BITXOR(_xlfn.BITXOR(_xlfn.BITXOR(_xlfn.BITXOR(_xlfn.BITXOR(L3,L4),L5),L6),L7),L8),L9),L10),L11),L12),L13),M3),M4),M5),M6),M7),M8),M9),M10),M11),M12),M13),2)</f>
+        <v>D2</v>
+      </c>
+      <c r="F16" s="23" t="str">
+        <f>DEC2HEX(MOD(SUM(L3:M13), 256))</f>
+        <v>94</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6">
+      <c r="E18" s="27" t="s">
+        <v>128</v>
+      </c>
+      <c r="F18" s="30" t="str">
+        <f>"0x"&amp;E16&amp;F16</f>
+        <v>0xD294</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6">
+      <c r="B19" s="31"/>
+    </row>
+    <row r="20" spans="2:6">
+      <c r="B20" s="32" t="s">
+        <v>130</v>
+      </c>
+      <c r="C20" s="32">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6">
+      <c r="B21" s="32" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6">
+      <c r="B22" s="32" t="s">
+        <v>132</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="SYaPsLKEBnA6CUzgiLuX96uHmJNqJmiwaVC/Gp7lCWlcbFB6o72rNe6ti1bJjBNaOcdwqptGkjV0elZBbg1urQ==" saltValue="UvkLaM+Q/FnHDuXv6yin3Q==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>